<commit_message>
update: soft_settings + database files
</commit_message>
<xml_diff>
--- a/soft_settings.xlsx
+++ b/soft_settings.xlsx
@@ -519,7 +519,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,17 +565,27 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>DAI</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>USDCe</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>USDT</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>USDC</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>USDCe</t>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>WETH</t>
         </is>
       </c>
     </row>

</xml_diff>